<commit_message>
Locust enemy added; heroes modified to attack enemy w/ pathways of land/air
</commit_message>
<xml_diff>
--- a/char descriptions.xlsx
+++ b/char descriptions.xlsx
@@ -225,12 +225,6 @@
     <t>just keep flying</t>
   </si>
   <si>
-    <t>Snails eats Slow Except for carrots and onions they love them.</t>
-  </si>
-  <si>
-    <t>They fairly likes all the fruits and vegetables.</t>
-  </si>
-  <si>
     <t>Surprise Surprise</t>
   </si>
   <si>
@@ -283,6 +277,12 @@
   </si>
   <si>
     <t>Looks like Mr. Hopper got a little tanned.</t>
+  </si>
+  <si>
+    <t>I'm a Slowpoke. Yep, no one cares.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They say i'm ugly. Just wait after my metamorphosis! </t>
   </si>
 </sst>
 </file>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -990,23 +990,23 @@
         <v>37</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1014,15 +1014,15 @@
         <v>38</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
starting to add the earth heroes on hero selected panel
</commit_message>
<xml_diff>
--- a/char descriptions.xlsx
+++ b/char descriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Character names</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Fruits &amp; Vegetables</t>
   </si>
   <si>
-    <t>King Guava</t>
-  </si>
-  <si>
-    <t>Queen Bittergourd</t>
-  </si>
-  <si>
     <t>Carrot</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Pests/Insects</t>
   </si>
   <si>
-    <t>Insect Queen (Angela)</t>
-  </si>
-  <si>
     <t>Ants</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t xml:space="preserve"> Description</t>
   </si>
   <si>
-    <t>King Guava is so  Guavable(Loveable) two queens from different got a crush on him.</t>
-  </si>
-  <si>
     <t>"ba ba ba ba ba nana"</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t xml:space="preserve">the Fruitties and Veggies are going Bananas over the heals </t>
   </si>
   <si>
-    <t>WaterMelon got some big seeds to talk about !</t>
-  </si>
-  <si>
     <t>This is the saucer that you cant eat !</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
     <t>Mega Cry!</t>
   </si>
   <si>
-    <t>A legendary web developer.</t>
-  </si>
-  <si>
     <t>This queen can get so INSECTcure sometimes !</t>
   </si>
   <si>
@@ -283,6 +265,9 @@
   </si>
   <si>
     <t>The first born of the Beetle brothers.</t>
+  </si>
+  <si>
+    <t>This dude  got some big seeds to talk about !</t>
   </si>
 </sst>
 </file>
@@ -686,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -701,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -711,161 +696,153 @@
       <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -874,187 +851,183 @@
     </row>
     <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" s="10"/>
     </row>
     <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>62</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">

</xml_diff>